<commit_message>
Scripts for the testing suite
</commit_message>
<xml_diff>
--- a/Examples/Experiment/Sapphire/TestDataBase.xlsx
+++ b/Examples/Experiment/Sapphire/TestDataBase.xlsx
@@ -4,26 +4,23 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="1" windowWidth="19200" windowHeight="8320"/>
+    <workbookView activeTab="0" windowWidth="12800" windowHeight="8030"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="1" r:id="rId1"/>
-    <sheet name="Sapphire" sheetId="2" r:id="rId2"/>
-    <sheet name="Sapphire-Lee" sheetId="3" r:id="rId3"/>
-    <sheet name="Silicon" sheetId="4" r:id="rId4"/>
-    <sheet name="6H-SiC" sheetId="5" r:id="rId5"/>
+    <sheet name="Sapphire-Lee" sheetId="2" r:id="rId2"/>
+    <sheet name="Silicon" sheetId="3" r:id="rId3"/>
+    <sheet name="6H-SiC" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Sheet_Title" localSheetId="0">"Information"</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">#REF!</definedName>
-    <definedName name="_xlnm.Sheet_Title" localSheetId="1">"Sapphire"</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="1">"Sapphire-Lee"</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">#REF!</definedName>
-    <definedName name="_xlnm.Sheet_Title" localSheetId="2">"Sapphire-Lee"</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="2">"Silicon"</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">#REF!</definedName>
-    <definedName name="_xlnm.Sheet_Title" localSheetId="3">"Silicon"</definedName>
+    <definedName name="_xlnm.Sheet_Title" localSheetId="3">"6H-SiC"</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">#REF!</definedName>
-    <definedName name="_xlnm.Sheet_Title" localSheetId="4">"6H-SiC"</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="4">#REF!</definedName>
   </definedNames>
   <calcPr calcMode="auto" iterate="1" iterateCount="100" iterateDelta="0.001"/>
   <webPublishing allowPng="1" css="0" codePage="1252"/>
@@ -84,10 +81,13 @@
     <t>Drude-Lorentz</t>
   </si>
   <si>
+    <t>FPSQ</t>
+  </si>
+  <si>
     <t>Direction</t>
   </si>
   <si>
-    <t>Eps0</t>
+    <t>Eps_inf</t>
   </si>
   <si>
     <t>Omega TO</t>
@@ -100,9 +100,6 @@
   </si>
   <si>
     <t>Gamma LO</t>
-  </si>
-  <si>
-    <t>FPSQ</t>
   </si>
   <si>
     <t>xx</t>
@@ -240,8 +237,8 @@
   </sheetPr>
   <dimension ref="A1:XFD43"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView workbookViewId="0" tabSelected="1">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="12.75"/>
@@ -498,6 +495,11 @@
     <row r="37" spans="1:16384">
       <c r="B37" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16384" ht="15">
+      <c r="B38" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:16384">
@@ -524,10 +526,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="67.5" defaultRowHeight="12.75"/>
@@ -543,28 +545,28 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G1" t="s">
         <v>1</v>
       </c>
       <c r="H1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -575,19 +577,19 @@
         <v>24</v>
       </c>
       <c r="B2">
-        <v>3.077</v>
+        <v>3.0499999999999998</v>
       </c>
       <c r="C2" s="3">
-        <v>384.99000000000001</v>
+        <v>384</v>
       </c>
       <c r="D2" s="4">
-        <v>3.2999999999999998</v>
+        <v>3.8999999999999999</v>
       </c>
       <c r="E2" s="3">
-        <v>387.60000000000002</v>
+        <v>387.19999999999999</v>
       </c>
       <c r="F2" s="4">
-        <v>3.1000000000000001</v>
+        <v>4</v>
       </c>
       <c r="G2" t="s">
         <v>3</v>
@@ -602,16 +604,16 @@
     </row>
     <row r="3" spans="1:14" ht="16.5">
       <c r="C3" s="3">
-        <v>439.10000000000002</v>
+        <v>438.5</v>
       </c>
       <c r="D3" s="4">
-        <v>3.1000000000000001</v>
+        <v>3.5</v>
       </c>
       <c r="E3" s="3">
-        <v>481.68000000000001</v>
+        <v>481.5</v>
       </c>
       <c r="F3" s="4">
-        <v>1.8999999999999999</v>
+        <v>3.7000000000000002</v>
       </c>
       <c r="G3" t="s">
         <v>9</v>
@@ -628,16 +630,16 @@
     </row>
     <row r="4" spans="1:14" ht="16.5">
       <c r="C4" s="5">
-        <v>569</v>
+        <v>568.5</v>
       </c>
       <c r="D4" s="6">
-        <v>4.7000000000000002</v>
+        <v>4.2000000000000002</v>
       </c>
       <c r="E4" s="3">
-        <v>629.5</v>
+        <v>629.10000000000002</v>
       </c>
       <c r="F4" s="4">
-        <v>5.9000000000000004</v>
+        <v>7</v>
       </c>
       <c r="G4" t="s">
         <v>10</v>
@@ -656,16 +658,16 @@
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="5">
-        <v>633.63</v>
+        <v>634</v>
       </c>
       <c r="D5" s="4">
-        <v>5</v>
+        <v>6.7999999999999998</v>
       </c>
       <c r="E5" s="3">
-        <v>906.60000000000002</v>
+        <v>907.5</v>
       </c>
       <c r="F5" s="4">
-        <v>14.699999999999999</v>
+        <v>17.800000000000001</v>
       </c>
       <c r="G5" t="s">
         <v>11</v>
@@ -681,20 +683,20 @@
       <c r="A6" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="2">
-        <v>3.077</v>
+      <c r="B6">
+        <v>3.0499999999999998</v>
       </c>
       <c r="C6" s="3">
-        <v>384.99000000000001</v>
+        <v>384</v>
       </c>
       <c r="D6" s="4">
-        <v>3.2999999999999998</v>
+        <v>3.8999999999999999</v>
       </c>
       <c r="E6" s="3">
-        <v>387.60000000000002</v>
+        <v>387.19999999999999</v>
       </c>
       <c r="F6" s="4">
-        <v>3.1000000000000001</v>
+        <v>4</v>
       </c>
       <c r="G6" t="s">
         <v>12</v>
@@ -709,18 +711,17 @@
     </row>
     <row r="7" spans="1:14" ht="16.5">
       <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
       <c r="C7" s="3">
-        <v>439.10000000000002</v>
+        <v>438.5</v>
       </c>
       <c r="D7" s="4">
-        <v>3.1000000000000001</v>
+        <v>3.5</v>
       </c>
       <c r="E7" s="3">
-        <v>481.68000000000001</v>
+        <v>481.5</v>
       </c>
       <c r="F7" s="4">
-        <v>1.8999999999999999</v>
+        <v>3.7000000000000002</v>
       </c>
       <c r="G7" t="s">
         <v>13</v>
@@ -735,18 +736,17 @@
     </row>
     <row r="8" spans="1:14" ht="16.5">
       <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
       <c r="C8" s="5">
-        <v>569</v>
+        <v>568.5</v>
       </c>
       <c r="D8" s="6">
-        <v>4.7000000000000002</v>
+        <v>4.2000000000000002</v>
       </c>
       <c r="E8" s="3">
-        <v>629.5</v>
+        <v>629.10000000000002</v>
       </c>
       <c r="F8" s="4">
-        <v>5.9000000000000004</v>
+        <v>7</v>
       </c>
       <c r="G8" t="s">
         <v>14</v>
@@ -763,16 +763,16 @@
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="5">
-        <v>633.63</v>
+        <v>634</v>
       </c>
       <c r="D9" s="4">
-        <v>5</v>
+        <v>6.7999999999999998</v>
       </c>
       <c r="E9" s="3">
-        <v>906.60000000000002</v>
+        <v>907.5</v>
       </c>
       <c r="F9" s="4">
-        <v>14.699999999999999</v>
+        <v>17.800000000000001</v>
       </c>
       <c r="G9" t="s">
         <v>4</v>
@@ -790,13 +790,13 @@
         <v>29</v>
       </c>
       <c r="B10" s="2">
-        <v>3.0720000000000001</v>
+        <v>3.0099999999999998</v>
       </c>
       <c r="C10" s="3">
-        <v>397.51999999999998</v>
+        <v>396</v>
       </c>
       <c r="D10" s="4">
-        <v>5.2999999999999998</v>
+        <v>1</v>
       </c>
       <c r="E10" s="3">
         <v>510.87</v>
@@ -820,7 +820,7 @@
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="3">
-        <v>582.40999999999997</v>
+        <v>582</v>
       </c>
       <c r="D11" s="4">
         <v>3</v>
@@ -871,13 +871,27 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>M.Schubert, T.E. Tiwlad, C.M. Herzinger, Phys Rev B Vol 61 (2000) 8187</t>
+          <t>S.C. Lee, S.S. Ng, H. Abu Hassan, Z. Hassan, T. Dumelow</t>
         </is>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="1:14" ht="15">
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Crystal orientation dependence of polarized infrared reflectance response of hexagonal sapphire crystal</t>
+        </is>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="15">
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Optical Materials (2014) vol 37, 773-779</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
@@ -896,363 +910,102 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:XFD7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="67.5" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" style="0" width="12.856370192307693"/>
-    <col min="3" max="3" style="0" width="12.140625" customWidth="1"/>
-    <col min="4" max="4" style="0" width="10.28515625" customWidth="1"/>
-    <col min="5" max="5" style="0" width="14.5703125" customWidth="1"/>
-    <col min="6" max="13" style="0" width="12.856370192307693"/>
-    <col min="14" max="14" style="0" width="14.5703125" customWidth="1"/>
-    <col min="15" max="16384" style="0" width="12.856370192307693"/>
+    <col min="1" max="16384" style="2" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15">
-      <c r="A1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>22</v>
+    <row r="1" spans="1:16384">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>cm-1</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Microns</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>k</t>
+        </is>
       </c>
       <c r="G1" t="s">
         <v>1</v>
       </c>
       <c r="H1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-    </row>
-    <row r="2" spans="1:14" ht="16.5">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2">
-        <v>3.0499999999999998</v>
-      </c>
-      <c r="C2" s="3">
-        <v>384</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16384">
+      <c r="C2" s="4">
+        <v>3.4199999999999999</v>
       </c>
       <c r="D2" s="4">
-        <v>3.8999999999999999</v>
-      </c>
-      <c r="E2" s="3">
-        <v>387.19999999999999</v>
-      </c>
-      <c r="F2" s="4">
-        <v>4</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E2" s="4"/>
       <c r="G2" t="s">
         <v>3</v>
       </c>
       <c r="H2">
-        <v>3.98</v>
-      </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="N2" s="3"/>
-    </row>
-    <row r="3" spans="1:14" ht="16.5">
-      <c r="C3" s="3">
-        <v>438.5</v>
-      </c>
-      <c r="D3" s="4">
-        <v>3.5</v>
-      </c>
-      <c r="E3" s="3">
-        <v>481.5</v>
-      </c>
-      <c r="F3" s="4">
-        <v>3.7000000000000002</v>
-      </c>
+        <v>2.3300000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16384">
       <c r="G3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3">
-        <v>4.7605000000000004</v>
-      </c>
-      <c r="I3" s="2"/>
-      <c r="J3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="2"/>
-      <c r="N3" s="3"/>
-    </row>
-    <row r="4" spans="1:14" ht="16.5">
-      <c r="C4" s="5">
-        <v>568.5</v>
-      </c>
-      <c r="D4" s="6">
-        <v>4.2000000000000002</v>
-      </c>
-      <c r="E4" s="3">
-        <v>629.10000000000002</v>
-      </c>
-      <c r="F4" s="4">
+        <v>4</v>
+      </c>
+      <c r="H3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16384">
+      <c r="G4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <f>MIN(A2:A618)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16384">
+      <c r="G5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5">
+        <f>MAX(A2:A618)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16384">
+      <c r="G6" t="s">
         <v>7</v>
       </c>
-      <c r="G4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4">
-        <v>4.7605000000000004</v>
-      </c>
-      <c r="I4" s="2"/>
-      <c r="J4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K4" s="2"/>
-      <c r="N4" s="3"/>
-    </row>
-    <row r="5" spans="1:14" ht="16.5">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="5">
-        <v>634</v>
-      </c>
-      <c r="D5" s="4">
-        <v>6.7999999999999998</v>
-      </c>
-      <c r="E5" s="3">
-        <v>907.5</v>
-      </c>
-      <c r="F5" s="4">
-        <v>17.800000000000001</v>
-      </c>
-      <c r="G5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5">
-        <v>12.9956</v>
-      </c>
-      <c r="I5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="N5" s="3"/>
-    </row>
-    <row r="6" spans="1:14" ht="16.5">
-      <c r="A6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6">
-        <v>3.0499999999999998</v>
-      </c>
-      <c r="C6" s="3">
-        <v>384</v>
-      </c>
-      <c r="D6" s="4">
-        <v>3.8999999999999999</v>
-      </c>
-      <c r="E6" s="3">
-        <v>387.19999999999999</v>
-      </c>
-      <c r="F6" s="4">
-        <v>4</v>
-      </c>
-      <c r="G6" t="s">
-        <v>12</v>
-      </c>
       <c r="H6">
-        <v>90</v>
-      </c>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="N6" s="3"/>
-    </row>
-    <row r="7" spans="1:14" ht="16.5">
-      <c r="A7" s="2"/>
-      <c r="C7" s="3">
-        <v>438.5</v>
-      </c>
-      <c r="D7" s="4">
-        <v>3.5</v>
-      </c>
-      <c r="E7" s="3">
-        <v>481.5</v>
-      </c>
-      <c r="F7" s="4">
-        <v>3.7000000000000002</v>
-      </c>
+        <f>COUNT(A2:A618)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16384">
       <c r="G7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7">
-        <v>90</v>
-      </c>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="N7" s="3"/>
-    </row>
-    <row r="8" spans="1:14" ht="16.5">
-      <c r="A8" s="2"/>
-      <c r="C8" s="5">
-        <v>568.5</v>
-      </c>
-      <c r="D8" s="6">
-        <v>4.2000000000000002</v>
-      </c>
-      <c r="E8" s="3">
-        <v>629.10000000000002</v>
-      </c>
-      <c r="F8" s="4">
-        <v>7</v>
-      </c>
-      <c r="G8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8">
-        <v>120</v>
-      </c>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="N8" s="3"/>
-    </row>
-    <row r="9" spans="1:14" ht="16.5">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="5">
-        <v>634</v>
-      </c>
-      <c r="D9" s="4">
-        <v>6.7999999999999998</v>
-      </c>
-      <c r="E9" s="3">
-        <v>907.5</v>
-      </c>
-      <c r="F9" s="4">
-        <v>17.800000000000001</v>
-      </c>
-      <c r="G9" t="s">
-        <v>4</v>
-      </c>
-      <c r="H9" t="s">
-        <v>28</v>
-      </c>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="N9" s="3"/>
-    </row>
-    <row r="10" spans="1:14" ht="16.5">
-      <c r="A10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="2">
-        <v>3.0099999999999998</v>
-      </c>
-      <c r="C10" s="3">
-        <v>396</v>
-      </c>
-      <c r="D10" s="4">
-        <v>1</v>
-      </c>
-      <c r="E10" s="3">
-        <v>510.87</v>
-      </c>
-      <c r="F10" s="4">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G10" t="s">
-        <v>5</v>
-      </c>
-      <c r="H10">
-        <f>MIN(A5:A621)</f>
-        <v>0</v>
-      </c>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="N10" s="3"/>
-    </row>
-    <row r="11" spans="1:14" ht="16.5">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="3">
-        <v>582</v>
-      </c>
-      <c r="D11" s="4">
-        <v>3</v>
-      </c>
-      <c r="E11" s="3">
-        <v>881.10000000000002</v>
-      </c>
-      <c r="F11" s="4">
-        <v>15.4</v>
-      </c>
-      <c r="G11" t="s">
-        <v>6</v>
-      </c>
-      <c r="H11">
-        <f>MAX(A5:A621)</f>
-        <v>0</v>
-      </c>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="N11" s="3"/>
-    </row>
-    <row r="12" spans="1:14" ht="15">
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" t="s">
-        <v>7</v>
-      </c>
-      <c r="H12">
-        <f>COUNT(A5:A621)</f>
-        <v>0</v>
-      </c>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="N12" s="2"/>
-    </row>
-    <row r="13" spans="1:14" ht="15">
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" t="s">
         <v>8</v>
       </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>S.C. Lee, S.S. Ng, H. Abu Hassan, Z. Hassan, T. Dumelow</t>
-        </is>
-      </c>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="N13" s="2"/>
-    </row>
-    <row r="14" spans="1:14" ht="15">
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>Crystal orientation dependence of polarized infrared reflectance response of hexagonal sapphire crystal</t>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>D . F . Edwards, in Handbook of Optical Constants of Solids, edited by E. D. Palik (Academic, Orlando, 1985), pp. 547-569.</t>
         </is>
       </c>
     </row>
@@ -1273,126 +1026,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:XFD7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="16384" style="2" width="12.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16384">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>cm-1</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Microns</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>n</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>k</t>
-        </is>
-      </c>
-      <c r="G1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16384">
-      <c r="C2" s="4">
-        <v>3.4199999999999999</v>
-      </c>
-      <c r="D2" s="4">
-        <v>0</v>
-      </c>
-      <c r="E2" s="4"/>
-      <c r="G2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2">
-        <v>2.3300000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16384">
-      <c r="G3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16384">
-      <c r="G4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4">
-        <f>MIN(A2:A618)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16384">
-      <c r="G5" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5">
-        <f>MAX(A2:A618)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16384">
-      <c r="G6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6">
-        <f>COUNT(A2:A618)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16384">
-      <c r="G7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>D . F . Edwards, in Handbook of Optical Constants of Solids, edited by E. D. Palik (Academic, Orlando, 1985), pp. 547-569.</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
-  <printOptions/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup blackAndWhite="0" cellComments="asDisplayed" draft="0" errors="displayed" fitToHeight="0" fitToWidth="0" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0"/>
-  <headerFooter>
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:gnmx="http://www.gnumeric.org/ext/spreadsheetml">
-  <sheetPr>
-    <pageSetUpPr fitToPage="0"/>
-  </sheetPr>
   <dimension ref="A1:XFD13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:K13"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15"/>
@@ -1404,7 +1041,7 @@
   <sheetData>
     <row r="1" spans="1:16384">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B1" t="inlineStr">
         <is>

</xml_diff>